<commit_message>
spreadsheets: Fix Organisation Type
The options were too long, and the last one was getting truncated
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation_v004.xlsx
+++ b/indigo/spreadsheetform_guides/organisation_v004.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sources" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="LanguageCodeOptions" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="CountryCodeOptions" sheetId="7" state="hidden" r:id="rId8"/>
+    <sheet name="TypeOptions" sheetId="8" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="395">
   <si>
     <t xml:space="preserve">INDIGO Organisation ID</t>
   </si>
@@ -1184,6 +1185,33 @@
   </si>
   <si>
     <t xml:space="preserve">ZW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered company, partnership or commercial association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered non-profit organisation, charity or foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilateral, bilateral or intergovernmental body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrangement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crowdfunding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unregistered organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collective</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1718,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11" type="list">
-      <formula1>"Registered company or partnership or commercial association,Registered non-profit organisation or charity or foundation,Government body,Multilateral or bilateral or intergovernmental body,Arrangement,Crowdfunding,Unregistered organisation,Individual,Colle"</formula1>
+      <formula1>TypeOptions!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4752,4 +4780,77 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>